<commit_message>
feat: remove print logs
</commit_message>
<xml_diff>
--- a/pkg/parser/testdata/cash_withdrawal_v2.xlsx
+++ b/pkg/parser/testdata/cash_withdrawal_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renth\FOR_FUN_PROJECTS\fork\firefly-iii-privatbank-importer\pkg\parser\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAB11ADD-924B-44F5-BE25-2C8606758817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5041FA61-82EF-4B10-8534-BE3D1A579041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27780" yWindow="600" windowWidth="25665" windowHeight="20505" xr2:uid="{8A539C5D-CEC0-4686-9DF8-9859E970CC74}"/>
+    <workbookView xWindow="1950" yWindow="1095" windowWidth="25665" windowHeight="20505" xr2:uid="{8A539C5D-CEC0-4686-9DF8-9859E970CC74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Data transakcji</t>
   </si>
@@ -97,6 +97,9 @@
   <si>
     <t>Konto Osobiste
 11111111111111111111111111</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -157,6 +160,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -496,16 +502,16 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="114" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45353</v>
       </c>
@@ -563,8 +569,8 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4">
-        <v>1.11111111111111E+25</v>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>

</xml_diff>